<commit_message>
removed extra files from 2015
</commit_message>
<xml_diff>
--- a/SIHadmissionDataset/2015/ORCR2015.xlsx
+++ b/SIHadmissionDataset/2015/ORCR2015.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7334" uniqueCount="2175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7336" uniqueCount="2177">
   <si>
     <r>
       <rPr>
@@ -7366,6 +7366,12 @@
   </si>
   <si>
     <t>SubCategory</t>
+  </si>
+  <si>
+    <t>OS:OTHERSTATE</t>
+  </si>
+  <si>
+    <t>HS:HOMESTATE</t>
   </si>
 </sst>
 </file>
@@ -7889,10 +7895,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K1803"/>
+  <dimension ref="A1:K1805"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A1789" workbookViewId="0">
+      <selection activeCell="A1805" sqref="A1805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -71008,6 +71014,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1804" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1804" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1805" t="s">
+        <v>2176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>